<commit_message>
Change -tap water- to Water Urban 3000 to 3300 to avoid upward collision
</commit_message>
<xml_diff>
--- a/data/ontology/2022-11-28_mfd-habitat-ontology.xlsx
+++ b/data/ontology/2022-11-28_mfd-habitat-ontology.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="241">
   <si>
     <t xml:space="preserve">mfd_sampletype</t>
   </si>
@@ -709,28 +709,40 @@
     <t xml:space="preserve">Groundwater</t>
   </si>
   <si>
+    <t xml:space="preserve">Harbours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wastewater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Influent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activated sludge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandfilter</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drinking water</t>
   </si>
   <si>
-    <t xml:space="preserve">Tap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterworks stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wastewater</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Influent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harbours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activated sludge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandfilter</t>
+    <t xml:space="preserve">tap water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterworks stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uncleaned/raw water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sandfilter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filtered water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treated water</t>
   </si>
 </sst>
 </file>
@@ -741,7 +753,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -783,10 +795,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF10D0C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -834,7 +854,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -864,6 +884,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -942,7 +966,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFF10D0C"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -956,10 +980,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K180"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G54" activeCellId="0" sqref="G54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G197" activeCellId="0" sqref="G197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5476,26 +5500,22 @@
         <v>227</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
       <c r="C175" s="7" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D175" s="7" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="E175" s="7" t="n">
-        <v>3100</v>
+        <v>1100</v>
       </c>
       <c r="F175" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G175" s="7" t="n">
-        <v>3110</v>
-      </c>
-      <c r="H175" s="7" t="s">
-        <v>230</v>
-      </c>
+      <c r="G175" s="7"/>
+      <c r="H175" s="7"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="7" t="s">
@@ -5511,13 +5531,13 @@
         <v>169</v>
       </c>
       <c r="E176" s="7" t="n">
-        <v>3100</v>
+        <v>3200</v>
       </c>
       <c r="F176" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G176" s="7" t="n">
-        <v>3120</v>
+        <v>3210</v>
       </c>
       <c r="H176" s="7" t="s">
         <v>231</v>
@@ -5540,42 +5560,38 @@
         <v>3200</v>
       </c>
       <c r="F177" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G177" s="7" t="n">
+        <v>3211</v>
+      </c>
+      <c r="H177" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="G177" s="7" t="n">
-        <v>3210</v>
-      </c>
-      <c r="H177" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="7" t="s">
         <v>227</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="C178" s="7" t="n">
         <v>1000</v>
       </c>
       <c r="D178" s="7" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E178" s="7" t="n">
         <v>1100</v>
       </c>
       <c r="F178" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="G178" s="7" t="n">
-        <v>1110</v>
-      </c>
-      <c r="H178" s="7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>233</v>
+      </c>
+      <c r="G178" s="7"/>
+      <c r="H178" s="7"/>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="7" t="s">
         <v>227</v>
       </c>
@@ -5585,20 +5601,8 @@
       <c r="C179" s="7" t="n">
         <v>3000</v>
       </c>
-      <c r="D179" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E179" s="7" t="n">
-        <v>3200</v>
-      </c>
-      <c r="F179" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="G179" s="7" t="n">
-        <v>3211</v>
-      </c>
-      <c r="H179" s="7" t="s">
-        <v>235</v>
+      <c r="D179" s="8" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5609,20 +5613,148 @@
         <v>169</v>
       </c>
       <c r="C180" s="7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D180" s="7" t="s">
+        <v>3000</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E180" s="8" t="n">
+        <v>3300</v>
+      </c>
+      <c r="F180" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="G180" s="8"/>
+      <c r="H180" s="8"/>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B181" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="E180" s="7" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F180" s="7" t="s">
+      <c r="C181" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D181" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E181" s="8" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F181" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="G180" s="7"/>
-      <c r="H180" s="7"/>
-    </row>
+      <c r="G181" s="8"/>
+      <c r="H181" s="8"/>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C182" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D182" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E182" s="8" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F182" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="G182" s="8" t="n">
+        <v>3110</v>
+      </c>
+      <c r="H182" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C183" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E183" s="8" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F183" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="G183" s="8" t="n">
+        <v>3120</v>
+      </c>
+      <c r="H183" s="8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C184" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E184" s="8" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F184" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="G184" s="8" t="n">
+        <v>3130</v>
+      </c>
+      <c r="H184" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C185" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D185" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="E185" s="8" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F185" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="G185" s="8" t="n">
+        <v>3140</v>
+      </c>
+      <c r="H185" s="8" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="G24:G122">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>

</xml_diff>